<commit_message>
Add water flow and piezo data
</commit_message>
<xml_diff>
--- a/water/Ebro/stations_selection.xlsx
+++ b/water/Ebro/stations_selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadevigo-my.sharepoint.com/personal/xurxo_rigueira_uvigo_gal/Documents/1_Ph.D/1_Code/data/water/Ebro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="989" documentId="1_{81DF0114-FEDC-4198-8515-1A051D1DD3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EAE54D6-6577-4794-8091-4AED7CEA1EBC}"/>
+  <xr:revisionPtr revIDLastSave="991" documentId="1_{81DF0114-FEDC-4198-8515-1A051D1DD3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21D07B7-FA99-4888-BFDB-C4DF612FBF70}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anos" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,9 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00C3C8E3-EFB9-401E-9D6A-16EA6D1B6E41}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Formato fechas: 'dd-mm-aaaa hh:mm:ss</t>
       </text>
     </comment>
@@ -554,7 +554,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -848,19 +848,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE83493-F446-42E8-90DC-AC38F245014F}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="D410" sqref="D410"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="91.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -874,7 +874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>901</v>
       </c>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>901</v>
       </c>
@@ -902,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>901</v>
       </c>
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>901</v>
       </c>
@@ -930,7 +930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>901</v>
       </c>
@@ -944,7 +944,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>901</v>
       </c>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>901</v>
       </c>
@@ -972,7 +972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>901</v>
       </c>
@@ -986,7 +986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>901</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>901</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>901</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>901</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>901</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>901</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>901</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>901</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>901</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>901</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>901</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>901</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>901</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>901</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>901</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>901</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>901</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>901</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>901</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>901</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>901</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>901</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>901</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>901</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>901</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>901</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>901</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>901</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>901</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>901</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>901</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>901</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>901</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>901</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>901</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>901</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>901</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>901</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>901</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>901</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>901</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>901</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>901</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>902</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>902</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>902</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>902</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>902</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>902</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>902</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>902</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>902</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>905</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>905</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>905</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>905</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>905</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>905</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>905</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <v>905</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>905</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <v>905</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>905</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>905</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>905</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>905</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <v>905</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>905</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>905</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>905</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <v>905</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>905</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>905</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>905</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <v>905</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <v>905</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>905</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>905</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>905</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>905</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>905</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>905</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>905</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>905</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>905</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>905</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>905</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>905</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>905</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>905</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>905</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>905</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>905</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <v>905</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>905</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>905</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>905</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>905</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>905</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>905</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>905</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>905</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>905</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>905</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>905</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>905</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>905</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>905</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>905</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>905</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>905</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>905</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>905</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>905</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>905</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>905</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>905</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>905</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>905</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>905</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <v>906</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>906</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>906</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>906</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>906</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>906</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>906</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>906</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>906</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>907</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>907</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>907</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>907</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>907</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>907</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>907</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>907</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>907</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>907</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>907</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>907</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="12">
         <v>907</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="12">
         <v>907</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="12">
         <v>907</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="12">
         <v>907</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="12">
         <v>907</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="12">
         <v>907</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="12">
         <v>907</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="12">
         <v>907</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="12">
         <v>907</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="12">
         <v>907</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="12">
         <v>907</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="12">
         <v>907</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="12">
         <v>907</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="12">
         <v>907</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="12">
         <v>907</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="12">
         <v>907</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="12">
         <v>907</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="12">
         <v>907</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>907</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>907</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>907</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>907</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>907</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>907</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>907</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>907</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>907</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="8">
         <v>907</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>907</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="8">
         <v>907</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <v>907</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="8">
         <v>910</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="8">
         <v>910</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="184" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="8">
         <v>910</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>910</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>910</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="8">
         <v>904</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="188" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="8">
         <v>904</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="8">
         <v>904</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="8">
         <v>904</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="8">
         <v>904</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="8">
         <v>904</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="8">
         <v>904</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="8">
         <v>904</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>904</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>904</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>904</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>904</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>904</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>904</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>904</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>904</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>904</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>904</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="8">
         <v>904</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>904</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>904</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>904</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>904</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>904</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="8">
         <v>904</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>904</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>904</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>904</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>904</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="8">
         <v>904</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>904</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="8">
         <v>904</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>904</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>904</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>904</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>904</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>904</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>904</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>904</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>904</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>904</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>904</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>904</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>904</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>904</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>904</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>904</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>904</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>904</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>904</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>904</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>904</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>904</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>904</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>904</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>904</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>904</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="12">
         <v>904</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="12">
         <v>904</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>904</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>904</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>904</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>904</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>904</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>904</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>904</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>904</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>904</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>904</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>904</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>904</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>904</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>904</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>904</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>904</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>904</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>904</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>904</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="8">
         <v>904</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>904</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>904</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="8">
         <v>904</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="8">
         <v>904</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>904</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>904</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>904</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="8">
         <v>904</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>904</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>904</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>904</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>904</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>904</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="8">
         <v>904</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="8">
         <v>904</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="8">
         <v>904</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="8">
         <v>904</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="8">
         <v>904</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>904</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>904</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>904</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" s="8">
         <v>904</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" s="8">
         <v>904</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>904</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>904</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>904</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" s="8">
         <v>904</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>904</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" s="8">
         <v>904</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" s="8">
         <v>904</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>904</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" s="8">
         <v>904</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" s="8">
         <v>904</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" s="8">
         <v>904</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" s="8">
         <v>904</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>904</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>904</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>904</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>904</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" s="8">
         <v>904</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" s="8">
         <v>904</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" s="8">
         <v>904</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" s="8">
         <v>904</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309" s="8">
         <v>904</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310" s="8">
         <v>904</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311" s="8">
         <v>904</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312" s="8">
         <v>904</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" s="8">
         <v>904</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314" s="8">
         <v>904</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" s="8">
         <v>904</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" s="8">
         <v>904</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" s="8">
         <v>904</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" s="8">
         <v>904</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" s="8">
         <v>904</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" s="8">
         <v>904</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321" s="8">
         <v>904</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322" s="8">
         <v>904</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323" s="8">
         <v>904</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" s="8">
         <v>904</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325" s="8">
         <v>904</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" s="8">
         <v>904</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327" s="8">
         <v>904</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>904</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" s="8">
         <v>904</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>904</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331" s="8">
         <v>904</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332" s="8">
         <v>904</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333" s="8">
         <v>904</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334" s="8">
         <v>904</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335" s="8">
         <v>904</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" s="8">
         <v>904</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337" s="8">
         <v>904</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338" s="8">
         <v>904</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339" s="8">
         <v>904</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340" s="8">
         <v>904</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341" s="8">
         <v>904</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342" s="8">
         <v>904</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343" s="8">
         <v>904</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344" s="8">
         <v>904</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345" s="8">
         <v>904</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346" s="8">
         <v>904</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347" s="8">
         <v>904</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348" s="8">
         <v>904</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" s="8">
         <v>904</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350" s="8">
         <v>904</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351" s="8">
         <v>904</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352" s="8">
         <v>904</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A353" s="8">
         <v>904</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354" s="8">
         <v>904</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A355" s="8">
         <v>904</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356" s="8">
         <v>904</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357" s="8">
         <v>904</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358" s="8">
         <v>904</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359" s="8">
         <v>904</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A360" s="8">
         <v>904</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361" s="8">
         <v>904</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A362" s="8">
         <v>904</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363" s="8">
         <v>904</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364" s="8">
         <v>904</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A365" s="8">
         <v>904</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A366" s="8">
         <v>904</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A367" s="8">
         <v>904</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A368" s="8">
         <v>904</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A369" s="8">
         <v>904</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A370" s="8">
         <v>904</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A371" s="8">
         <v>904</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A372" s="8">
         <v>904</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A373" s="8">
         <v>904</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A374" s="8">
         <v>904</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A375" s="8">
         <v>904</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A376" s="8">
         <v>904</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A377" s="8">
         <v>904</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A378" s="8">
         <v>904</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A379" s="8">
         <v>904</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A380" s="8">
         <v>904</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A381" s="8">
         <v>904</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A382" s="8">
         <v>904</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A383" s="8">
         <v>904</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A384" s="8">
         <v>904</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A385" s="8">
         <v>904</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A386" s="8">
         <v>904</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387" s="8">
         <v>904</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388" s="8">
         <v>904</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A389" s="8">
         <v>904</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" s="8">
         <v>904</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A391" s="8">
         <v>904</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A392" s="8">
         <v>904</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393" s="8">
         <v>904</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394" s="8">
         <v>904</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A395" s="8">
         <v>904</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A396" s="8">
         <v>904</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A397" s="8">
         <v>904</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A398" s="8">
         <v>904</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399" s="8">
         <v>904</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400" s="8">
         <v>904</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A401" s="8">
         <v>904</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A402" s="8">
         <v>904</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A403" s="8">
         <v>904</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>904</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A405" s="8">
         <v>904</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>913</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>913</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>913</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A409" s="8">
         <v>916</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>916</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>916</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A412" s="8">
         <v>916</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>916</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A414" s="1">
         <v>916</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A415" s="1">
         <v>916</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A416" s="1">
         <v>916</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A417" s="1">
         <v>916</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418" s="1">
         <v>916</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A419" s="1">
         <v>916</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>916</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>916</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A422" s="1">
         <v>916</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
         <v>916</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
         <v>916</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>916</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A426" s="1">
         <v>916</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427" s="8">
         <v>916</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
         <v>916</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>916</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>916</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>916</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>916</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>916</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>916</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>916</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436" s="8">
         <v>916</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="437" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>916</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>916</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="439" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>916</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="440" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>916</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="441" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441" s="1">
         <v>916</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="442" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442" s="1">
         <v>916</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>916</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="444" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444" s="8">
         <v>916</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="445" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445" s="1">
         <v>916</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="446" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446" s="8">
         <v>916</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="447" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447" s="1">
         <v>916</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="448" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448" s="1">
         <v>916</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449" s="8">
         <v>916</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450" s="1">
         <v>916</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="451" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451" s="1">
         <v>916</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="452" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452" s="1">
         <v>916</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="453" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453" s="1">
         <v>916</v>
       </c>
@@ -7220,20 +7220,20 @@
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="1"/>
-    <col min="4" max="4" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="1"/>
-    <col min="8" max="8" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" style="1"/>
+    <col min="8" max="8" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>901</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>902</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>903</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>904</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>905</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>906</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>907</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>908</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>909</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>910</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>911</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>912</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>913</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>914</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>916</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>918</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>919</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>920</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>921</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>922</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>924</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>926</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>927</v>
       </c>
@@ -7545,7 +7545,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>928</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>929</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>930</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>950</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>951</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>952</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>961</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>963</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>965</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>966</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>968</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>969</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>970</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>980</v>
       </c>

</xml_diff>